<commit_message>
fifth commit expenses page is added
</commit_message>
<xml_diff>
--- a/SignUp_Data.xlsx
+++ b/SignUp_Data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -218,9 +219,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -229,32 +230,26 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -266,19 +261,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -291,90 +337,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,37 +390,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,145 +564,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,6 +599,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -613,35 +638,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -653,6 +649,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,165 +686,161 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1170,7 +1171,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="2"/>
@@ -1344,10 +1345,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.40625" customWidth="1"/>
-    <col min="2" max="2" width="17.4453125" customWidth="1"/>
-    <col min="3" max="3" width="30.8515625" customWidth="1"/>
-    <col min="4" max="4" width="18.09375" customWidth="1"/>
+    <col min="1" max="1" width="16.40625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.4453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.8515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.09375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1597,4 +1598,20 @@
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel file for login function is added
</commit_message>
<xml_diff>
--- a/SignUp_Data.xlsx
+++ b/SignUp_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="2">
   <si>
     <t>email</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>Andreacci</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -224,9 +230,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -1182,10 +1188,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="30.3359375" customWidth="1"/>
-    <col min="2" max="2" width="20.4375" customWidth="1"/>
-    <col min="3" max="3" width="14.3203125" customWidth="1"/>
-    <col min="4" max="4" width="11.984375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.3359375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.4375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.3203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1206,7 +1212,9 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
@@ -1215,7 +1223,9 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
@@ -1224,7 +1234,9 @@
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
@@ -1233,7 +1245,9 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
@@ -1242,7 +1256,9 @@
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
@@ -1251,7 +1267,9 @@
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
@@ -1260,7 +1278,9 @@
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
@@ -1269,7 +1289,9 @@
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
@@ -1278,7 +1300,9 @@
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
@@ -1287,7 +1311,9 @@
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
@@ -1296,7 +1322,9 @@
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
@@ -1305,7 +1333,9 @@
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
@@ -1314,7 +1344,9 @@
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
@@ -1323,7 +1355,9 @@
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
@@ -1332,7 +1366,9 @@
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
@@ -1341,7 +1377,9 @@
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1363,10 +1401,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.40625" customWidth="1"/>
-    <col min="2" max="2" width="17.4453125" customWidth="1"/>
-    <col min="3" max="3" width="30.8515625" customWidth="1"/>
-    <col min="4" max="4" width="18.09375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.40625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.4453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.8515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.09375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
login and signup tests are done
</commit_message>
<xml_diff>
--- a/SignUp_Data.xlsx
+++ b/SignUp_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27020" windowHeight="12360"/>
+    <workbookView windowWidth="27020" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
   <si>
     <t>email</t>
   </si>
@@ -33,6 +33,9 @@
     <t>TwBcPP</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>ahaccleton1@va.gov</t>
   </si>
   <si>
@@ -123,6 +126,9 @@
     <t>duobank</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -219,10 +225,16 @@
     <t>Andreacci</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t>panddreaccie@jalbum.net</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>Pdutnam</t>
+  </si>
+  <si>
+    <t>panddddreaccie@jalbum.net</t>
   </si>
 </sst>
 </file>
@@ -230,10 +242,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -242,15 +254,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,7 +286,89 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,84 +383,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -377,21 +404,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -402,73 +414,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,109 +576,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,41 +626,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -669,6 +648,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -679,6 +673,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,159 +714,157 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1182,16 +1194,16 @@
   <sheetPr/>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.3359375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.4375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.3203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.984375" collapsed="true"/>
+    <col min="1" max="1" width="30.3359375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.4375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.3203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1213,172 +1225,172 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1393,26 +1405,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:E16"/>
+    <sheetView showOutlineSymbols="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.40625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.4453125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.8515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.09375" collapsed="true"/>
+    <col min="1" max="1" width="16.40625" customWidth="1"/>
+    <col min="2" max="2" width="17.4453125" customWidth="1"/>
+    <col min="3" max="3" width="30.8515625" customWidth="1"/>
+    <col min="4" max="4" width="18.09375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1426,10 +1438,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1437,219 +1449,290 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" display="panddreaccie@jalbum.net"/>
+    <hyperlink ref="C18" r:id="rId2" display="panddddreaccie@jalbum.net" tooltip="mailto:panddddreaccie@jalbum.net"/>
+    <hyperlink ref="C5" r:id="rId3" display="tmacrannell3@mashable.com"/>
+    <hyperlink ref="C6" r:id="rId4" display="gandrzej4@forbes.com"/>
+    <hyperlink ref="C7" r:id="rId5" display="spearman5@t-online.de"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
expenses tests are done
</commit_message>
<xml_diff>
--- a/SignUp_Data.xlsx
+++ b/SignUp_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="0">
   <si>
     <t>email</t>
   </si>
@@ -141,30 +141,45 @@
     <t>Widmore</t>
   </si>
   <si>
+    <t>fwidemore0@shareasale.com</t>
+  </si>
+  <si>
     <t>Annabel</t>
   </si>
   <si>
     <t>Haccleton</t>
   </si>
   <si>
+    <t>ahacecleton1@va.gov</t>
+  </si>
+  <si>
     <t>Tiphany</t>
   </si>
   <si>
     <t>Schapero</t>
   </si>
   <si>
+    <t>tschapeero2@woothemes.com</t>
+  </si>
+  <si>
     <t>Travers</t>
   </si>
   <si>
     <t>MacRannell</t>
   </si>
   <si>
+    <t>tmacreanenell3@mashable.com</t>
+  </si>
+  <si>
     <t>Gina</t>
   </si>
   <si>
     <t>Andrzej</t>
   </si>
   <si>
+    <t>ganderzej4@forbes.com</t>
+  </si>
+  <si>
     <t>Sigfried</t>
   </si>
   <si>
@@ -177,24 +192,36 @@
     <t>Malser</t>
   </si>
   <si>
+    <t>rmalseer6@webmd.com</t>
+  </si>
+  <si>
     <t>Gratia</t>
   </si>
   <si>
     <t>Janew</t>
   </si>
   <si>
+    <t>gjeanew7@newsvine.com</t>
+  </si>
+  <si>
     <t>Sigrid</t>
   </si>
   <si>
     <t>Zannotelli</t>
   </si>
   <si>
+    <t>szanenotelli8@sitemeter.com</t>
+  </si>
+  <si>
     <t>Chrissie</t>
   </si>
   <si>
     <t>Da Costa</t>
   </si>
   <si>
+    <t>cdeacosta9@virginia.edu</t>
+  </si>
+  <si>
     <t>Suzanna</t>
   </si>
   <si>
@@ -219,6 +246,9 @@
     <t>Spellman</t>
   </si>
   <si>
+    <t>bspeellmand@elegantthemes.com</t>
+  </si>
+  <si>
     <t>Putnam</t>
   </si>
   <si>
@@ -228,13 +258,16 @@
     <t>panddreaccie@jalbum.net</t>
   </si>
   <si>
-    <t>dddd</t>
+    <t>ww</t>
   </si>
   <si>
     <t>Pdutnam</t>
   </si>
   <si>
     <t>panddddreaccie@jalbum.net</t>
+  </si>
+  <si>
+    <t>cccccss442</t>
   </si>
 </sst>
 </file>
@@ -242,10 +275,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -254,6 +287,35 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -262,8 +324,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,9 +334,76 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -285,13 +415,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -300,47 +423,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -351,59 +437,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -414,187 +447,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,15 +656,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -643,6 +667,33 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -677,26 +728,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -714,157 +745,159 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1200,10 +1233,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="30.3359375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.4375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.3203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.984375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.3359375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.4375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.3203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1280,7 +1313,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1408,15 +1441,15 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showOutlineSymbols="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C2:C8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.40625" customWidth="1"/>
-    <col min="2" max="2" width="17.4453125" customWidth="1"/>
-    <col min="3" max="3" width="30.8515625" customWidth="1"/>
-    <col min="4" max="4" width="18.09375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.40625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.4453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.8515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.09375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1444,24 +1477,24 @@
         <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1472,13 +1505,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -1489,44 +1522,44 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -1540,13 +1573,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>17</v>
@@ -1557,13 +1590,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -1574,30 +1607,30 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>23</v>
@@ -1608,10 +1641,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
@@ -1620,15 +1653,15 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
@@ -1642,10 +1675,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -1659,13 +1692,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>31</v>
@@ -1676,10 +1709,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1688,50 +1721,58 @@
         <v>33</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" t="s">
-        <v>36</v>
+        <v>82</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" display="panddreaccie@jalbum.net"/>
     <hyperlink ref="C18" r:id="rId2" display="panddddreaccie@jalbum.net" tooltip="mailto:panddddreaccie@jalbum.net"/>
-    <hyperlink ref="C5" r:id="rId3" display="tmacrannell3@mashable.com"/>
-    <hyperlink ref="C6" r:id="rId4" display="gandrzej4@forbes.com"/>
+    <hyperlink ref="C5" r:id="rId3" display="tmacreanenell3@mashable.com" tooltip="mailto:tmacreanenell3@mashable.com"/>
+    <hyperlink ref="C6" r:id="rId4" display="ganderzej4@forbes.com" tooltip="mailto:ganderzej4@forbes.com"/>
     <hyperlink ref="C7" r:id="rId5" display="spearman5@t-online.de"/>
+    <hyperlink ref="C2" r:id="rId6" display="fwidemore0@shareasale.com"/>
+    <hyperlink ref="C3" r:id="rId7" display="ahacecleton1@va.gov"/>
+    <hyperlink ref="C4" r:id="rId8" display="tschapeero2@woothemes.com"/>
+    <hyperlink ref="C8" r:id="rId9" display="rmalseer6@webmd.com"/>
+    <hyperlink ref="C9" r:id="rId10" display="gjeanew7@newsvine.com"/>
+    <hyperlink ref="C11" r:id="rId11" display="cdeacosta9@virginia.edu"/>
+    <hyperlink ref="C10" r:id="rId12" display="szanenotelli8@sitemeter.com"/>
+    <hyperlink ref="C15" r:id="rId13" display="bspeellmand@elegantthemes.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
failed tests are updated
</commit_message>
<xml_diff>
--- a/SignUp_Data.xlsx
+++ b/SignUp_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="0">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="0">
   <si>
     <t>email</t>
   </si>
@@ -1280,7 +1280,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1368,7 +1368,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1379,7 +1379,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1390,7 +1390,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1412,7 +1412,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3">

</xml_diff>